<commit_message>
- remove unittest_config and move functionality to sqlite_util_test - fix all tests
</commit_message>
<xml_diff>
--- a/excel-app/files/database new.xlsx
+++ b/excel-app/files/database new.xlsx
@@ -854,8 +854,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -940,8 +940,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>